<commit_message>
add UAT kelompok 10
</commit_message>
<xml_diff>
--- a/UAT (kelompok 10).xlsx
+++ b/UAT (kelompok 10).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>ID Tes</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Status (Pass/Fail)</t>
   </si>
   <si>
+    <t xml:space="preserve">KELOMPOK 10 : </t>
+  </si>
+  <si>
     <t>TC-01</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>PASS</t>
   </si>
   <si>
+    <t>1. KEN ABEL VALLERON LIMANSYAH - C14210227</t>
+  </si>
+  <si>
     <t>TC-02</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t>Tetap di halaman Login, muncul flash message "Login Gagal".</t>
+  </si>
+  <si>
+    <t>2. JASON ENRICO SANTOSO - C14210067</t>
   </si>
   <si>
     <t>TC-03</t>
@@ -233,7 +242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -241,6 +250,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -274,12 +295,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -508,6 +535,7 @@
     <col customWidth="1" min="4" max="4" width="37.88"/>
     <col customWidth="1" min="5" max="5" width="39.88"/>
     <col customWidth="1" min="6" max="6" width="48.0"/>
+    <col customWidth="1" min="9" max="9" width="50.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="63.0" customHeight="1">
@@ -532,258 +560,267 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="61.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="62.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" ht="60.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="77.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" ht="76.5" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" ht="64.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" ht="60.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" ht="66.0" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" ht="65.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" ht="76.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" ht="79.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>